<commit_message>
successfully writing new estimate with job number and client name
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10107"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA323925-F370-8D4B-975E-F970935D8ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6637BB45-E0D6-5345-982A-E3A4C2AD956D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45700" yWindow="-16340" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -617,6 +617,61 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -638,63 +693,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1041,7 +1041,7 @@
   <dimension ref="A1:L80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1061,30 +1061,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="45" t="s">
+      <c r="I1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="47"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="66"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="50"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="69"/>
     </row>
     <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
@@ -1122,8 +1122,8 @@
       <c r="H6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="51"/>
-      <c r="J6" s="52"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="46"/>
     </row>
     <row r="7" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="11"/>
@@ -1138,14 +1138,14 @@
       <c r="F8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="51" t="s">
+      <c r="G8" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="52"/>
-      <c r="I8" s="53" t="s">
+      <c r="H8" s="46"/>
+      <c r="I8" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="54"/>
+      <c r="J8" s="70"/>
       <c r="K8" s="13">
         <v>2022</v>
       </c>
@@ -1163,18 +1163,18 @@
       <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="55" t="s">
+      <c r="C10" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="53" t="s">
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="58"/>
+      <c r="J10" s="60"/>
       <c r="K10" s="12" t="s">
         <v>17</v>
       </c>
@@ -1191,15 +1191,15 @@
       <c r="B12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="51" t="s">
+      <c r="C12" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="52"/>
+      <c r="D12" s="46"/>
       <c r="F12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="59"/>
-      <c r="H12" s="52"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="46"/>
       <c r="I12" s="11"/>
       <c r="J12" s="5"/>
       <c r="K12" s="4"/>
@@ -1210,15 +1210,15 @@
       <c r="B14" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="60" t="s">
+      <c r="C14" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="62"/>
-      <c r="H14" s="62"/>
-      <c r="I14" s="62"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
       <c r="J14" s="15" t="s">
         <v>23</v>
       </c>
@@ -1395,9 +1395,9 @@
     </row>
     <row r="27" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="4"/>
-      <c r="C27" s="63"/>
-      <c r="D27" s="63"/>
-      <c r="E27" s="63"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="55"/>
       <c r="F27" s="7"/>
       <c r="H27" s="4"/>
     </row>
@@ -1416,11 +1416,11 @@
       <c r="C29" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="64" t="s">
+      <c r="D29" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="E29" s="64"/>
-      <c r="F29" s="64"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
       <c r="G29" s="23" t="s">
         <v>27</v>
       </c>
@@ -1451,11 +1451,11 @@
       <c r="C31" s="13">
         <v>2185</v>
       </c>
-      <c r="D31" s="65" t="s">
+      <c r="D31" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="E31" s="65"/>
-      <c r="F31" s="65"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
       <c r="G31" s="26"/>
       <c r="H31" s="26"/>
       <c r="I31" s="26"/>
@@ -1470,11 +1470,11 @@
       <c r="C32" s="13">
         <v>3762</v>
       </c>
-      <c r="D32" s="66" t="s">
+      <c r="D32" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="E32" s="67"/>
-      <c r="F32" s="52"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="46"/>
       <c r="G32" s="26"/>
       <c r="H32" s="26"/>
       <c r="I32" s="26"/>
@@ -1489,11 +1489,11 @@
       <c r="C33" s="13">
         <v>863</v>
       </c>
-      <c r="D33" s="65" t="s">
+      <c r="D33" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="E33" s="65"/>
-      <c r="F33" s="65"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="47"/>
       <c r="G33" s="26"/>
       <c r="H33" s="28"/>
       <c r="I33" s="26"/>
@@ -1508,11 +1508,11 @@
       <c r="C34" s="12">
         <v>2330</v>
       </c>
-      <c r="D34" s="65" t="s">
+      <c r="D34" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="E34" s="65"/>
-      <c r="F34" s="65"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="47"/>
       <c r="G34" s="26"/>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -1527,11 +1527,11 @@
       <c r="C35" s="12">
         <v>136</v>
       </c>
-      <c r="D35" s="66" t="s">
+      <c r="D35" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="E35" s="68"/>
-      <c r="F35" s="69"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="54"/>
       <c r="G35" s="26"/>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -1546,11 +1546,11 @@
       <c r="C36" s="13">
         <v>592</v>
       </c>
-      <c r="D36" s="66" t="s">
+      <c r="D36" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="E36" s="67"/>
-      <c r="F36" s="52"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="46"/>
       <c r="G36" s="26">
         <v>0</v>
       </c>
@@ -1567,11 +1567,11 @@
       <c r="C37" s="12">
         <v>524</v>
       </c>
-      <c r="D37" s="66" t="s">
+      <c r="D37" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="E37" s="67"/>
-      <c r="F37" s="52"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="46"/>
       <c r="G37" s="26"/>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -1586,11 +1586,11 @@
       <c r="C38" s="13">
         <v>696</v>
       </c>
-      <c r="D38" s="65" t="s">
+      <c r="D38" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E38" s="65"/>
-      <c r="F38" s="65"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="47"/>
       <c r="G38" s="26"/>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -1605,11 +1605,11 @@
       <c r="C39" s="13">
         <v>584</v>
       </c>
-      <c r="D39" s="66" t="s">
+      <c r="D39" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="E39" s="67"/>
-      <c r="F39" s="52"/>
+      <c r="E39" s="45"/>
+      <c r="F39" s="46"/>
       <c r="G39" s="26"/>
       <c r="H39" s="29"/>
       <c r="I39" s="26"/>
@@ -1624,11 +1624,11 @@
       <c r="C40" s="13">
         <v>564</v>
       </c>
-      <c r="D40" s="66" t="s">
+      <c r="D40" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="E40" s="68"/>
-      <c r="F40" s="69"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="54"/>
       <c r="G40" s="26"/>
       <c r="H40" s="26"/>
       <c r="I40" s="26"/>
@@ -1643,11 +1643,11 @@
       <c r="C41" s="13">
         <v>596</v>
       </c>
-      <c r="D41" s="66" t="s">
+      <c r="D41" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="E41" s="67"/>
-      <c r="F41" s="52"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="46"/>
       <c r="G41" s="26"/>
       <c r="H41" s="29"/>
       <c r="I41" s="26"/>
@@ -1662,11 +1662,11 @@
       <c r="C42" s="12">
         <v>2326</v>
       </c>
-      <c r="D42" s="66" t="s">
+      <c r="D42" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="E42" s="67"/>
-      <c r="F42" s="52"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="46"/>
       <c r="G42" s="26"/>
       <c r="H42" s="26"/>
       <c r="I42" s="26"/>
@@ -1681,11 +1681,11 @@
       <c r="C43" s="13">
         <v>676</v>
       </c>
-      <c r="D43" s="66" t="s">
+      <c r="D43" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="E43" s="68"/>
-      <c r="F43" s="69"/>
+      <c r="E43" s="53"/>
+      <c r="F43" s="54"/>
       <c r="G43" s="26"/>
       <c r="H43" s="26"/>
       <c r="I43" s="26"/>
@@ -1700,11 +1700,11 @@
       <c r="C44" s="13">
         <v>732</v>
       </c>
-      <c r="D44" s="66" t="s">
+      <c r="D44" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="E44" s="68"/>
-      <c r="F44" s="69"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="54"/>
       <c r="G44" s="26" t="s">
         <v>48</v>
       </c>
@@ -1721,11 +1721,11 @@
       <c r="C45" s="13">
         <v>720</v>
       </c>
-      <c r="D45" s="66" t="s">
+      <c r="D45" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="E45" s="68"/>
-      <c r="F45" s="69"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="54"/>
       <c r="G45" s="26"/>
       <c r="H45" s="26"/>
       <c r="I45" s="26"/>
@@ -1740,11 +1740,11 @@
       <c r="C46" s="13">
         <v>832</v>
       </c>
-      <c r="D46" s="66" t="s">
+      <c r="D46" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="E46" s="67"/>
-      <c r="F46" s="52"/>
+      <c r="E46" s="45"/>
+      <c r="F46" s="46"/>
       <c r="G46" s="26"/>
       <c r="H46" s="26"/>
       <c r="I46" s="26"/>
@@ -1759,11 +1759,11 @@
       <c r="C47" s="12">
         <v>520</v>
       </c>
-      <c r="D47" s="66" t="s">
+      <c r="D47" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="E47" s="67"/>
-      <c r="F47" s="52"/>
+      <c r="E47" s="45"/>
+      <c r="F47" s="46"/>
       <c r="G47" s="26"/>
       <c r="H47" s="26"/>
       <c r="I47" s="26"/>
@@ -1778,11 +1778,11 @@
       <c r="C48" s="13">
         <v>400</v>
       </c>
-      <c r="D48" s="65" t="s">
+      <c r="D48" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="E48" s="65"/>
-      <c r="F48" s="65"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="47"/>
       <c r="G48" s="26"/>
       <c r="H48" s="26"/>
       <c r="I48" s="26"/>
@@ -1797,11 +1797,11 @@
       <c r="C49" s="13">
         <v>737</v>
       </c>
-      <c r="D49" s="66" t="s">
+      <c r="D49" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="E49" s="68"/>
-      <c r="F49" s="69"/>
+      <c r="E49" s="53"/>
+      <c r="F49" s="54"/>
       <c r="G49" s="26"/>
       <c r="H49" s="26"/>
       <c r="I49" s="26"/>
@@ -1816,11 +1816,11 @@
       <c r="C50" s="12">
         <v>2437</v>
       </c>
-      <c r="D50" s="65" t="s">
+      <c r="D50" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="E50" s="65"/>
-      <c r="F50" s="65"/>
+      <c r="E50" s="47"/>
+      <c r="F50" s="47"/>
       <c r="G50" s="26"/>
       <c r="H50" s="26"/>
       <c r="I50" s="26"/>
@@ -1835,11 +1835,11 @@
       <c r="C51" s="12">
         <v>2394</v>
       </c>
-      <c r="D51" s="65" t="s">
+      <c r="D51" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="E51" s="65"/>
-      <c r="F51" s="65"/>
+      <c r="E51" s="47"/>
+      <c r="F51" s="47"/>
       <c r="G51" s="26"/>
       <c r="H51" s="26"/>
       <c r="I51" s="26"/>
@@ -1854,11 +1854,11 @@
       <c r="C52" s="13">
         <v>2192</v>
       </c>
-      <c r="D52" s="65" t="s">
+      <c r="D52" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="E52" s="65"/>
-      <c r="F52" s="65"/>
+      <c r="E52" s="47"/>
+      <c r="F52" s="47"/>
       <c r="G52" s="26"/>
       <c r="H52" s="26"/>
       <c r="I52" s="26"/>
@@ -1873,11 +1873,11 @@
       <c r="C53" s="13">
         <v>760</v>
       </c>
-      <c r="D53" s="65" t="s">
+      <c r="D53" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="E53" s="65"/>
-      <c r="F53" s="65"/>
+      <c r="E53" s="47"/>
+      <c r="F53" s="47"/>
       <c r="G53" s="26"/>
       <c r="H53" s="26"/>
       <c r="I53" s="26"/>
@@ -1892,11 +1892,11 @@
       <c r="C54" s="13">
         <v>792</v>
       </c>
-      <c r="D54" s="65" t="s">
+      <c r="D54" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="E54" s="65"/>
-      <c r="F54" s="65"/>
+      <c r="E54" s="47"/>
+      <c r="F54" s="47"/>
       <c r="G54" s="26"/>
       <c r="H54" s="26"/>
       <c r="I54" s="26"/>
@@ -1911,11 +1911,11 @@
       <c r="C55" s="12">
         <v>840</v>
       </c>
-      <c r="D55" s="65" t="s">
+      <c r="D55" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="E55" s="65"/>
-      <c r="F55" s="65"/>
+      <c r="E55" s="47"/>
+      <c r="F55" s="47"/>
       <c r="G55" s="26"/>
       <c r="H55" s="26"/>
       <c r="I55" s="26"/>
@@ -1930,11 +1930,11 @@
       <c r="C56" s="13">
         <v>500</v>
       </c>
-      <c r="D56" s="65" t="s">
+      <c r="D56" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="E56" s="65"/>
-      <c r="F56" s="65"/>
+      <c r="E56" s="47"/>
+      <c r="F56" s="47"/>
       <c r="G56" s="26">
         <v>50</v>
       </c>
@@ -1951,11 +1951,11 @@
       <c r="C57" s="13">
         <v>768</v>
       </c>
-      <c r="D57" s="65" t="s">
+      <c r="D57" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="E57" s="65"/>
-      <c r="F57" s="65"/>
+      <c r="E57" s="47"/>
+      <c r="F57" s="47"/>
       <c r="G57" s="26"/>
       <c r="H57" s="26"/>
       <c r="I57" s="26"/>
@@ -1970,11 +1970,11 @@
       <c r="C58" s="12">
         <v>2322</v>
       </c>
-      <c r="D58" s="66" t="s">
+      <c r="D58" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="E58" s="67"/>
-      <c r="F58" s="52"/>
+      <c r="E58" s="45"/>
+      <c r="F58" s="46"/>
       <c r="G58" s="26"/>
       <c r="H58" s="26"/>
       <c r="I58" s="26"/>
@@ -1985,9 +1985,9 @@
     <row r="59" spans="2:12" ht="15" x14ac:dyDescent="0.2">
       <c r="B59" s="13"/>
       <c r="C59" s="13"/>
-      <c r="D59" s="51"/>
-      <c r="E59" s="67"/>
-      <c r="F59" s="52"/>
+      <c r="D59" s="44"/>
+      <c r="E59" s="45"/>
+      <c r="F59" s="46"/>
       <c r="G59" s="26"/>
       <c r="H59" s="26"/>
       <c r="I59" s="26"/>
@@ -1996,11 +1996,11 @@
       <c r="L59" s="27"/>
     </row>
     <row r="60" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="D60" s="65" t="s">
+      <c r="D60" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="E60" s="65"/>
-      <c r="F60" s="65"/>
+      <c r="E60" s="47"/>
+      <c r="F60" s="47"/>
       <c r="G60" s="26">
         <f>SUM(G31:G58)</f>
         <v>50</v>
@@ -2219,18 +2219,53 @@
       <c r="B80" s="15"/>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
-      <c r="E80" s="60" t="s">
+      <c r="E80" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="F80" s="62"/>
-      <c r="G80" s="64"/>
-      <c r="H80" s="70"/>
-      <c r="I80" s="70"/>
+      <c r="F80" s="49"/>
+      <c r="G80" s="50"/>
+      <c r="H80" s="51"/>
+      <c r="I80" s="51"/>
       <c r="J80" s="4"/>
       <c r="K80" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="I1:L2"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C14:I14"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="D52:F52"/>
+    <mergeCell ref="D53:F53"/>
     <mergeCell ref="D59:F59"/>
     <mergeCell ref="D60:F60"/>
     <mergeCell ref="E80:F80"/>
@@ -2240,46 +2275,8 @@
     <mergeCell ref="D56:F56"/>
     <mergeCell ref="D57:F57"/>
     <mergeCell ref="D58:F58"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="D50:F50"/>
-    <mergeCell ref="D51:F51"/>
-    <mergeCell ref="D52:F52"/>
-    <mergeCell ref="D53:F53"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C14:I14"/>
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="I1:L2"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:J8"/>
   </mergeCells>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>"All TDA, CGO, DEN, NYR, KSC, TRI, POINT, TEXAS"</formula1>
-    </dataValidation>
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"All TDA, CGO, DEN, NYR, KSC, TRI, "</formula1>
     </dataValidation>

</xml_diff>